<commit_message>
Testes nas funções de movimentação
</commit_message>
<xml_diff>
--- a/bitmap_pacman.xlsx
+++ b/bitmap_pacman.xlsx
@@ -55,7 +55,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -101,13 +101,19 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFDF0902"/>
-        <bgColor rgb="FF993300"/>
+        <bgColor rgb="FFED1C24"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFA9893"/>
         <bgColor rgb="FFFF8080"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFED1C24"/>
+        <bgColor rgb="FFDF0902"/>
       </patternFill>
     </fill>
   </fills>
@@ -145,7 +151,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -183,6 +189,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -249,7 +259,7 @@
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FFED1C24"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
@@ -263,20 +273,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:BL32"/>
+  <dimension ref="A1:BL49"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="37" zoomScaleNormal="37" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AK22" activeCellId="0" sqref="AK22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J37" activeCellId="0" sqref="J37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="48" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="47.9" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="53" min="1" style="1" width="10"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="54" style="1" width="9.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="65" style="1" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="1" width="8.62"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="48" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="47.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="n">
         <v>0</v>
       </c>
@@ -533,7 +541,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="48" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="47.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="n">
         <f aca="false">A1+256</f>
         <v>256</v>
@@ -791,7 +799,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="48" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="47.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="n">
         <f aca="false">A2+256</f>
         <v>512</v>
@@ -1049,7 +1057,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="48" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="47.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="n">
         <f aca="false">A3+256</f>
         <v>768</v>
@@ -1307,7 +1315,7 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="48" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="47.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="n">
         <f aca="false">A4+256</f>
         <v>1024</v>
@@ -1565,7 +1573,7 @@
         <v>1276</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="48" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="47.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="n">
         <f aca="false">A5+256</f>
         <v>1280</v>
@@ -1823,7 +1831,7 @@
         <v>1532</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="48" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="47.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="n">
         <f aca="false">A6+256</f>
         <v>1536</v>
@@ -2081,7 +2089,7 @@
         <v>2300</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="48" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="47.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="n">
         <f aca="false">A7+256</f>
         <v>1792</v>
@@ -2339,7 +2347,7 @@
         <v>2044</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="48" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="47.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="n">
         <f aca="false">A8+256</f>
         <v>2048</v>
@@ -2597,7 +2605,7 @@
         <v>2300</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="48" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="47.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="n">
         <f aca="false">A9+256</f>
         <v>2304</v>
@@ -2855,7 +2863,7 @@
         <v>2556</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="48" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="47.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="n">
         <f aca="false">A10+256</f>
         <v>2560</v>
@@ -3113,7 +3121,7 @@
         <v>2812</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="48" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="47.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="n">
         <f aca="false">A11+256</f>
         <v>2816</v>
@@ -3371,7 +3379,7 @@
         <v>3068</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="48" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="47.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="n">
         <f aca="false">A12+256</f>
         <v>3072</v>
@@ -3629,7 +3637,7 @@
         <v>3324</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="48" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="47.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="n">
         <f aca="false">A13+256</f>
         <v>3328</v>
@@ -3887,7 +3895,7 @@
         <v>3580</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="48" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="47.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="n">
         <f aca="false">A14+256</f>
         <v>3584</v>
@@ -4145,7 +4153,7 @@
         <v>3836</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="48" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="47.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="n">
         <f aca="false">A15+256</f>
         <v>3840</v>
@@ -4403,7 +4411,7 @@
         <v>4092</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="48" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="47.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="n">
         <f aca="false">A16+256</f>
         <v>4096</v>
@@ -4661,7 +4669,7 @@
         <v>4348</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="48" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="47.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="n">
         <f aca="false">A17+256</f>
         <v>4352</v>
@@ -4919,7 +4927,7 @@
         <v>4604</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="48" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="47.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="n">
         <f aca="false">A18+256</f>
         <v>4608</v>
@@ -5177,7 +5185,7 @@
         <v>4860</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="48" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="47.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="n">
         <f aca="false">A19+256</f>
         <v>4864</v>
@@ -5435,7 +5443,7 @@
         <v>5116</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="48" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="47.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="n">
         <f aca="false">A20+256</f>
         <v>5120</v>
@@ -5693,7 +5701,7 @@
         <v>5372</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="48" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="47.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="n">
         <f aca="false">A21+256</f>
         <v>5376</v>
@@ -5951,7 +5959,7 @@
         <v>5628</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="48" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="47.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="n">
         <f aca="false">A22+256</f>
         <v>5632</v>
@@ -6209,7 +6217,7 @@
         <v>5884</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="48" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="47.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="n">
         <f aca="false">A23+256</f>
         <v>5888</v>
@@ -6467,7 +6475,7 @@
         <v>6140</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="48" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="47.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="n">
         <f aca="false">A24+256</f>
         <v>6144</v>
@@ -6725,7 +6733,7 @@
         <v>6396</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="48" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="47.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="n">
         <f aca="false">A25+256</f>
         <v>6400</v>
@@ -6983,7 +6991,7 @@
         <v>6652</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="48" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="47.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="n">
         <f aca="false">A26+256</f>
         <v>6656</v>
@@ -7241,7 +7249,7 @@
         <v>6908</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="48" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="47.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="n">
         <f aca="false">A27+256</f>
         <v>6912</v>
@@ -7499,7 +7507,7 @@
         <v>7164</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="48" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="47.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="n">
         <f aca="false">A28+256</f>
         <v>7168</v>
@@ -7757,7 +7765,7 @@
         <v>7420</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="48" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="47.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="n">
         <f aca="false">A29+256</f>
         <v>7424</v>
@@ -8015,7 +8023,7 @@
         <v>7676</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="48" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="47.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="n">
         <f aca="false">A30+256</f>
         <v>7680</v>
@@ -8273,7 +8281,7 @@
         <v>7932</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="48" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="47.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="n">
         <f aca="false">A31+256</f>
         <v>7936</v>
@@ -8529,6 +8537,2085 @@
       <c r="BL32" s="2" t="n">
         <f aca="false">BK32+4</f>
         <v>8188</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="47.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A34" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="B34" s="2" t="n">
+        <f aca="false">4+A34</f>
+        <v>4</v>
+      </c>
+      <c r="C34" s="2" t="n">
+        <f aca="false">4+B34</f>
+        <v>8</v>
+      </c>
+      <c r="D34" s="2" t="n">
+        <f aca="false">4+C34</f>
+        <v>12</v>
+      </c>
+      <c r="E34" s="2" t="n">
+        <f aca="false">4+D34</f>
+        <v>16</v>
+      </c>
+      <c r="F34" s="2" t="n">
+        <f aca="false">4+E34</f>
+        <v>20</v>
+      </c>
+      <c r="G34" s="2" t="n">
+        <f aca="false">4+F34</f>
+        <v>24</v>
+      </c>
+      <c r="H34" s="2" t="n">
+        <f aca="false">4+G34</f>
+        <v>28</v>
+      </c>
+      <c r="I34" s="2" t="n">
+        <f aca="false">4+H34</f>
+        <v>32</v>
+      </c>
+      <c r="J34" s="2" t="n">
+        <f aca="false">4+I34</f>
+        <v>36</v>
+      </c>
+      <c r="K34" s="2" t="n">
+        <f aca="false">4+J34</f>
+        <v>40</v>
+      </c>
+      <c r="L34" s="2" t="n">
+        <f aca="false">4+K34</f>
+        <v>44</v>
+      </c>
+      <c r="M34" s="2" t="n">
+        <f aca="false">4+L34</f>
+        <v>48</v>
+      </c>
+      <c r="N34" s="2" t="n">
+        <f aca="false">4+M34</f>
+        <v>52</v>
+      </c>
+      <c r="O34" s="2" t="n">
+        <f aca="false">4+N34</f>
+        <v>56</v>
+      </c>
+      <c r="P34" s="2" t="n">
+        <f aca="false">4+O34</f>
+        <v>60</v>
+      </c>
+      <c r="Q34" s="2" t="n">
+        <f aca="false">4+P34</f>
+        <v>64</v>
+      </c>
+      <c r="R34" s="2" t="n">
+        <f aca="false">4+Q34</f>
+        <v>68</v>
+      </c>
+      <c r="S34" s="2" t="n">
+        <f aca="false">4+R34</f>
+        <v>72</v>
+      </c>
+      <c r="T34" s="2" t="n">
+        <f aca="false">4+S34</f>
+        <v>76</v>
+      </c>
+      <c r="U34" s="2" t="n">
+        <f aca="false">4+T34</f>
+        <v>80</v>
+      </c>
+      <c r="V34" s="2" t="n">
+        <f aca="false">4+U34</f>
+        <v>84</v>
+      </c>
+      <c r="W34" s="2" t="n">
+        <f aca="false">4+V34</f>
+        <v>88</v>
+      </c>
+      <c r="X34" s="2" t="n">
+        <f aca="false">4+W34</f>
+        <v>92</v>
+      </c>
+      <c r="Y34" s="2" t="n">
+        <f aca="false">4+X34</f>
+        <v>96</v>
+      </c>
+      <c r="Z34" s="2" t="n">
+        <f aca="false">4+Y34</f>
+        <v>100</v>
+      </c>
+      <c r="AA34" s="2" t="n">
+        <f aca="false">4+Z34</f>
+        <v>104</v>
+      </c>
+      <c r="AB34" s="2" t="n">
+        <f aca="false">4+AA34</f>
+        <v>108</v>
+      </c>
+      <c r="AC34" s="2" t="n">
+        <f aca="false">4+AB34</f>
+        <v>112</v>
+      </c>
+      <c r="AD34" s="2" t="n">
+        <f aca="false">4+AC34</f>
+        <v>116</v>
+      </c>
+      <c r="AE34" s="2" t="n">
+        <f aca="false">4+AD34</f>
+        <v>120</v>
+      </c>
+      <c r="AF34" s="2" t="n">
+        <f aca="false">4+AE34</f>
+        <v>124</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="47.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A35" s="2" t="n">
+        <f aca="false">128+A34</f>
+        <v>128</v>
+      </c>
+      <c r="B35" s="4" t="n">
+        <f aca="false">4+A35</f>
+        <v>132</v>
+      </c>
+      <c r="C35" s="4" t="n">
+        <f aca="false">4+B35</f>
+        <v>136</v>
+      </c>
+      <c r="D35" s="4" t="n">
+        <f aca="false">4+C35</f>
+        <v>140</v>
+      </c>
+      <c r="E35" s="4" t="n">
+        <f aca="false">4+D35</f>
+        <v>144</v>
+      </c>
+      <c r="F35" s="4" t="n">
+        <f aca="false">4+E35</f>
+        <v>148</v>
+      </c>
+      <c r="G35" s="4" t="n">
+        <f aca="false">4+F35</f>
+        <v>152</v>
+      </c>
+      <c r="H35" s="4" t="n">
+        <f aca="false">4+G35</f>
+        <v>156</v>
+      </c>
+      <c r="I35" s="4" t="n">
+        <f aca="false">4+H35</f>
+        <v>160</v>
+      </c>
+      <c r="J35" s="4" t="n">
+        <f aca="false">4+I35</f>
+        <v>164</v>
+      </c>
+      <c r="K35" s="4" t="n">
+        <f aca="false">4+J35</f>
+        <v>168</v>
+      </c>
+      <c r="L35" s="4" t="n">
+        <f aca="false">4+K35</f>
+        <v>172</v>
+      </c>
+      <c r="M35" s="4" t="n">
+        <f aca="false">4+L35</f>
+        <v>176</v>
+      </c>
+      <c r="N35" s="4" t="n">
+        <f aca="false">4+M35</f>
+        <v>180</v>
+      </c>
+      <c r="O35" s="4" t="n">
+        <f aca="false">4+N35</f>
+        <v>184</v>
+      </c>
+      <c r="P35" s="2" t="n">
+        <f aca="false">4+O35</f>
+        <v>188</v>
+      </c>
+      <c r="Q35" s="2" t="n">
+        <f aca="false">4+P35</f>
+        <v>192</v>
+      </c>
+      <c r="R35" s="2" t="n">
+        <f aca="false">4+Q35</f>
+        <v>196</v>
+      </c>
+      <c r="S35" s="2" t="n">
+        <f aca="false">4+R35</f>
+        <v>200</v>
+      </c>
+      <c r="T35" s="2" t="n">
+        <f aca="false">4+S35</f>
+        <v>204</v>
+      </c>
+      <c r="U35" s="2" t="n">
+        <f aca="false">4+T35</f>
+        <v>208</v>
+      </c>
+      <c r="V35" s="2" t="n">
+        <f aca="false">4+U35</f>
+        <v>212</v>
+      </c>
+      <c r="W35" s="2" t="n">
+        <f aca="false">4+V35</f>
+        <v>216</v>
+      </c>
+      <c r="X35" s="2" t="n">
+        <f aca="false">4+W35</f>
+        <v>220</v>
+      </c>
+      <c r="Y35" s="2" t="n">
+        <f aca="false">4+X35</f>
+        <v>224</v>
+      </c>
+      <c r="Z35" s="2" t="n">
+        <f aca="false">4+Y35</f>
+        <v>228</v>
+      </c>
+      <c r="AA35" s="2" t="n">
+        <f aca="false">4+Z35</f>
+        <v>232</v>
+      </c>
+      <c r="AB35" s="2" t="n">
+        <f aca="false">4+AA35</f>
+        <v>236</v>
+      </c>
+      <c r="AC35" s="2" t="n">
+        <f aca="false">4+AB35</f>
+        <v>240</v>
+      </c>
+      <c r="AD35" s="2" t="n">
+        <f aca="false">4+AC35</f>
+        <v>244</v>
+      </c>
+      <c r="AE35" s="2" t="n">
+        <f aca="false">4+AD35</f>
+        <v>248</v>
+      </c>
+      <c r="AF35" s="2" t="n">
+        <f aca="false">4+AE35</f>
+        <v>252</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="47.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A36" s="2" t="n">
+        <f aca="false">128+A35</f>
+        <v>256</v>
+      </c>
+      <c r="B36" s="4" t="n">
+        <f aca="false">4+A36</f>
+        <v>260</v>
+      </c>
+      <c r="C36" s="2" t="n">
+        <f aca="false">4+B36</f>
+        <v>264</v>
+      </c>
+      <c r="D36" s="2" t="n">
+        <f aca="false">4+C36</f>
+        <v>268</v>
+      </c>
+      <c r="E36" s="2" t="n">
+        <f aca="false">4+D36</f>
+        <v>272</v>
+      </c>
+      <c r="F36" s="2" t="n">
+        <f aca="false">4+E36</f>
+        <v>276</v>
+      </c>
+      <c r="G36" s="2" t="n">
+        <f aca="false">4+F36</f>
+        <v>280</v>
+      </c>
+      <c r="H36" s="2" t="n">
+        <f aca="false">4+G36</f>
+        <v>284</v>
+      </c>
+      <c r="I36" s="2" t="n">
+        <f aca="false">4+H36</f>
+        <v>288</v>
+      </c>
+      <c r="J36" s="2" t="n">
+        <f aca="false">4+I36</f>
+        <v>292</v>
+      </c>
+      <c r="K36" s="2" t="n">
+        <f aca="false">4+J36</f>
+        <v>296</v>
+      </c>
+      <c r="L36" s="2" t="n">
+        <f aca="false">4+K36</f>
+        <v>300</v>
+      </c>
+      <c r="M36" s="2" t="n">
+        <f aca="false">4+L36</f>
+        <v>304</v>
+      </c>
+      <c r="N36" s="2" t="n">
+        <f aca="false">4+M36</f>
+        <v>308</v>
+      </c>
+      <c r="O36" s="4" t="n">
+        <f aca="false">4+N36</f>
+        <v>312</v>
+      </c>
+      <c r="P36" s="2" t="n">
+        <f aca="false">4+O36</f>
+        <v>316</v>
+      </c>
+      <c r="Q36" s="2" t="n">
+        <f aca="false">4+P36</f>
+        <v>320</v>
+      </c>
+      <c r="R36" s="2" t="n">
+        <f aca="false">4+Q36</f>
+        <v>324</v>
+      </c>
+      <c r="S36" s="2" t="n">
+        <f aca="false">4+R36</f>
+        <v>328</v>
+      </c>
+      <c r="T36" s="2" t="n">
+        <f aca="false">4+S36</f>
+        <v>332</v>
+      </c>
+      <c r="U36" s="2" t="n">
+        <f aca="false">4+T36</f>
+        <v>336</v>
+      </c>
+      <c r="V36" s="2" t="n">
+        <f aca="false">4+U36</f>
+        <v>340</v>
+      </c>
+      <c r="W36" s="2" t="n">
+        <f aca="false">4+V36</f>
+        <v>344</v>
+      </c>
+      <c r="X36" s="2" t="n">
+        <f aca="false">4+W36</f>
+        <v>348</v>
+      </c>
+      <c r="Y36" s="2" t="n">
+        <f aca="false">4+X36</f>
+        <v>352</v>
+      </c>
+      <c r="Z36" s="2" t="n">
+        <f aca="false">4+Y36</f>
+        <v>356</v>
+      </c>
+      <c r="AA36" s="2" t="n">
+        <f aca="false">4+Z36</f>
+        <v>360</v>
+      </c>
+      <c r="AB36" s="2" t="n">
+        <f aca="false">4+AA36</f>
+        <v>364</v>
+      </c>
+      <c r="AC36" s="2" t="n">
+        <f aca="false">4+AB36</f>
+        <v>368</v>
+      </c>
+      <c r="AD36" s="2" t="n">
+        <f aca="false">4+AC36</f>
+        <v>372</v>
+      </c>
+      <c r="AE36" s="2" t="n">
+        <f aca="false">4+AD36</f>
+        <v>376</v>
+      </c>
+      <c r="AF36" s="2" t="n">
+        <f aca="false">4+AE36</f>
+        <v>380</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="47.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A37" s="2" t="n">
+        <f aca="false">128+A36</f>
+        <v>384</v>
+      </c>
+      <c r="B37" s="4" t="n">
+        <f aca="false">4+A37</f>
+        <v>388</v>
+      </c>
+      <c r="C37" s="2" t="n">
+        <f aca="false">4+B37</f>
+        <v>392</v>
+      </c>
+      <c r="D37" s="10" t="n">
+        <f aca="false">4+C37</f>
+        <v>396</v>
+      </c>
+      <c r="E37" s="2" t="n">
+        <f aca="false">4+D37</f>
+        <v>400</v>
+      </c>
+      <c r="F37" s="2" t="n">
+        <f aca="false">4+E37</f>
+        <v>404</v>
+      </c>
+      <c r="G37" s="2" t="n">
+        <f aca="false">4+F37</f>
+        <v>408</v>
+      </c>
+      <c r="H37" s="2" t="n">
+        <f aca="false">4+G37</f>
+        <v>412</v>
+      </c>
+      <c r="I37" s="2" t="n">
+        <f aca="false">4+H37</f>
+        <v>416</v>
+      </c>
+      <c r="J37" s="2" t="n">
+        <f aca="false">4+I37</f>
+        <v>420</v>
+      </c>
+      <c r="K37" s="2" t="n">
+        <f aca="false">4+J37</f>
+        <v>424</v>
+      </c>
+      <c r="L37" s="2" t="n">
+        <f aca="false">4+K37</f>
+        <v>428</v>
+      </c>
+      <c r="M37" s="2" t="n">
+        <f aca="false">4+L37</f>
+        <v>432</v>
+      </c>
+      <c r="N37" s="2" t="n">
+        <f aca="false">4+M37</f>
+        <v>436</v>
+      </c>
+      <c r="O37" s="4" t="n">
+        <f aca="false">4+N37</f>
+        <v>440</v>
+      </c>
+      <c r="P37" s="2" t="n">
+        <f aca="false">4+O37</f>
+        <v>444</v>
+      </c>
+      <c r="Q37" s="2" t="n">
+        <f aca="false">4+P37</f>
+        <v>448</v>
+      </c>
+      <c r="R37" s="2" t="n">
+        <f aca="false">4+Q37</f>
+        <v>452</v>
+      </c>
+      <c r="S37" s="2" t="n">
+        <f aca="false">4+R37</f>
+        <v>456</v>
+      </c>
+      <c r="T37" s="2" t="n">
+        <f aca="false">4+S37</f>
+        <v>460</v>
+      </c>
+      <c r="U37" s="2" t="n">
+        <f aca="false">4+T37</f>
+        <v>464</v>
+      </c>
+      <c r="V37" s="2" t="n">
+        <f aca="false">4+U37</f>
+        <v>468</v>
+      </c>
+      <c r="W37" s="2" t="n">
+        <f aca="false">4+V37</f>
+        <v>472</v>
+      </c>
+      <c r="X37" s="2" t="n">
+        <f aca="false">4+W37</f>
+        <v>476</v>
+      </c>
+      <c r="Y37" s="2" t="n">
+        <f aca="false">4+X37</f>
+        <v>480</v>
+      </c>
+      <c r="Z37" s="2" t="n">
+        <f aca="false">4+Y37</f>
+        <v>484</v>
+      </c>
+      <c r="AA37" s="2" t="n">
+        <f aca="false">4+Z37</f>
+        <v>488</v>
+      </c>
+      <c r="AB37" s="2" t="n">
+        <f aca="false">4+AA37</f>
+        <v>492</v>
+      </c>
+      <c r="AC37" s="2" t="n">
+        <f aca="false">4+AB37</f>
+        <v>496</v>
+      </c>
+      <c r="AD37" s="2" t="n">
+        <f aca="false">4+AC37</f>
+        <v>500</v>
+      </c>
+      <c r="AE37" s="2" t="n">
+        <f aca="false">4+AD37</f>
+        <v>504</v>
+      </c>
+      <c r="AF37" s="2" t="n">
+        <f aca="false">4+AE37</f>
+        <v>508</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="47.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A38" s="2" t="n">
+        <f aca="false">128+A37</f>
+        <v>512</v>
+      </c>
+      <c r="B38" s="4" t="n">
+        <f aca="false">4+A38</f>
+        <v>516</v>
+      </c>
+      <c r="C38" s="2" t="n">
+        <f aca="false">4+B38</f>
+        <v>520</v>
+      </c>
+      <c r="D38" s="2" t="n">
+        <f aca="false">4+C38</f>
+        <v>524</v>
+      </c>
+      <c r="E38" s="2" t="n">
+        <f aca="false">4+D38</f>
+        <v>528</v>
+      </c>
+      <c r="F38" s="2" t="n">
+        <f aca="false">4+E38</f>
+        <v>532</v>
+      </c>
+      <c r="G38" s="2" t="n">
+        <f aca="false">4+F38</f>
+        <v>536</v>
+      </c>
+      <c r="H38" s="2" t="n">
+        <f aca="false">4+G38</f>
+        <v>540</v>
+      </c>
+      <c r="I38" s="2" t="n">
+        <f aca="false">4+H38</f>
+        <v>544</v>
+      </c>
+      <c r="J38" s="2" t="n">
+        <f aca="false">4+I38</f>
+        <v>548</v>
+      </c>
+      <c r="K38" s="2" t="n">
+        <f aca="false">4+J38</f>
+        <v>552</v>
+      </c>
+      <c r="L38" s="2" t="n">
+        <f aca="false">4+K38</f>
+        <v>556</v>
+      </c>
+      <c r="M38" s="2" t="n">
+        <f aca="false">4+L38</f>
+        <v>560</v>
+      </c>
+      <c r="N38" s="2" t="n">
+        <f aca="false">4+M38</f>
+        <v>564</v>
+      </c>
+      <c r="O38" s="4" t="n">
+        <f aca="false">4+N38</f>
+        <v>568</v>
+      </c>
+      <c r="P38" s="2" t="n">
+        <f aca="false">4+O38</f>
+        <v>572</v>
+      </c>
+      <c r="Q38" s="2" t="n">
+        <f aca="false">4+P38</f>
+        <v>576</v>
+      </c>
+      <c r="R38" s="2" t="n">
+        <f aca="false">4+Q38</f>
+        <v>580</v>
+      </c>
+      <c r="S38" s="2" t="n">
+        <f aca="false">4+R38</f>
+        <v>584</v>
+      </c>
+      <c r="T38" s="2" t="n">
+        <f aca="false">4+S38</f>
+        <v>588</v>
+      </c>
+      <c r="U38" s="2" t="n">
+        <f aca="false">4+T38</f>
+        <v>592</v>
+      </c>
+      <c r="V38" s="2" t="n">
+        <f aca="false">4+U38</f>
+        <v>596</v>
+      </c>
+      <c r="W38" s="2" t="n">
+        <f aca="false">4+V38</f>
+        <v>600</v>
+      </c>
+      <c r="X38" s="2" t="n">
+        <f aca="false">4+W38</f>
+        <v>604</v>
+      </c>
+      <c r="Y38" s="2" t="n">
+        <f aca="false">4+X38</f>
+        <v>608</v>
+      </c>
+      <c r="Z38" s="2" t="n">
+        <f aca="false">4+Y38</f>
+        <v>612</v>
+      </c>
+      <c r="AA38" s="2" t="n">
+        <f aca="false">4+Z38</f>
+        <v>616</v>
+      </c>
+      <c r="AB38" s="2" t="n">
+        <f aca="false">4+AA38</f>
+        <v>620</v>
+      </c>
+      <c r="AC38" s="2" t="n">
+        <f aca="false">4+AB38</f>
+        <v>624</v>
+      </c>
+      <c r="AD38" s="2" t="n">
+        <f aca="false">4+AC38</f>
+        <v>628</v>
+      </c>
+      <c r="AE38" s="2" t="n">
+        <f aca="false">4+AD38</f>
+        <v>632</v>
+      </c>
+      <c r="AF38" s="2" t="n">
+        <f aca="false">4+AE38</f>
+        <v>636</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="47.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A39" s="2" t="n">
+        <f aca="false">128+A38</f>
+        <v>640</v>
+      </c>
+      <c r="B39" s="4" t="n">
+        <f aca="false">4+A39</f>
+        <v>644</v>
+      </c>
+      <c r="C39" s="2" t="n">
+        <f aca="false">4+B39</f>
+        <v>648</v>
+      </c>
+      <c r="D39" s="2" t="n">
+        <f aca="false">4+C39</f>
+        <v>652</v>
+      </c>
+      <c r="E39" s="2" t="n">
+        <f aca="false">4+D39</f>
+        <v>656</v>
+      </c>
+      <c r="F39" s="2" t="n">
+        <f aca="false">4+E39</f>
+        <v>660</v>
+      </c>
+      <c r="G39" s="2" t="n">
+        <f aca="false">4+F39</f>
+        <v>664</v>
+      </c>
+      <c r="H39" s="2" t="n">
+        <f aca="false">4+G39</f>
+        <v>668</v>
+      </c>
+      <c r="I39" s="2" t="n">
+        <f aca="false">4+H39</f>
+        <v>672</v>
+      </c>
+      <c r="J39" s="2" t="n">
+        <f aca="false">4+I39</f>
+        <v>676</v>
+      </c>
+      <c r="K39" s="2" t="n">
+        <f aca="false">4+J39</f>
+        <v>680</v>
+      </c>
+      <c r="L39" s="2" t="n">
+        <f aca="false">4+K39</f>
+        <v>684</v>
+      </c>
+      <c r="M39" s="2" t="n">
+        <f aca="false">4+L39</f>
+        <v>688</v>
+      </c>
+      <c r="N39" s="2" t="n">
+        <f aca="false">4+M39</f>
+        <v>692</v>
+      </c>
+      <c r="O39" s="4" t="n">
+        <f aca="false">4+N39</f>
+        <v>696</v>
+      </c>
+      <c r="P39" s="2" t="n">
+        <f aca="false">4+O39</f>
+        <v>700</v>
+      </c>
+      <c r="Q39" s="2" t="n">
+        <f aca="false">4+P39</f>
+        <v>704</v>
+      </c>
+      <c r="R39" s="2" t="n">
+        <f aca="false">4+Q39</f>
+        <v>708</v>
+      </c>
+      <c r="S39" s="2" t="n">
+        <f aca="false">4+R39</f>
+        <v>712</v>
+      </c>
+      <c r="T39" s="2" t="n">
+        <f aca="false">4+S39</f>
+        <v>716</v>
+      </c>
+      <c r="U39" s="2" t="n">
+        <f aca="false">4+T39</f>
+        <v>720</v>
+      </c>
+      <c r="V39" s="2" t="n">
+        <f aca="false">4+U39</f>
+        <v>724</v>
+      </c>
+      <c r="W39" s="2" t="n">
+        <f aca="false">4+V39</f>
+        <v>728</v>
+      </c>
+      <c r="X39" s="2" t="n">
+        <f aca="false">4+W39</f>
+        <v>732</v>
+      </c>
+      <c r="Y39" s="2" t="n">
+        <f aca="false">4+X39</f>
+        <v>736</v>
+      </c>
+      <c r="Z39" s="2" t="n">
+        <f aca="false">4+Y39</f>
+        <v>740</v>
+      </c>
+      <c r="AA39" s="2" t="n">
+        <f aca="false">4+Z39</f>
+        <v>744</v>
+      </c>
+      <c r="AB39" s="2" t="n">
+        <f aca="false">4+AA39</f>
+        <v>748</v>
+      </c>
+      <c r="AC39" s="2" t="n">
+        <f aca="false">4+AB39</f>
+        <v>752</v>
+      </c>
+      <c r="AD39" s="2" t="n">
+        <f aca="false">4+AC39</f>
+        <v>756</v>
+      </c>
+      <c r="AE39" s="2" t="n">
+        <f aca="false">4+AD39</f>
+        <v>760</v>
+      </c>
+      <c r="AF39" s="2" t="n">
+        <f aca="false">4+AE39</f>
+        <v>764</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="47.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A40" s="2" t="n">
+        <f aca="false">128+A39</f>
+        <v>768</v>
+      </c>
+      <c r="B40" s="4" t="n">
+        <f aca="false">4+A40</f>
+        <v>772</v>
+      </c>
+      <c r="C40" s="2" t="n">
+        <f aca="false">4+B40</f>
+        <v>776</v>
+      </c>
+      <c r="D40" s="2" t="n">
+        <f aca="false">4+C40</f>
+        <v>780</v>
+      </c>
+      <c r="E40" s="2" t="n">
+        <f aca="false">4+D40</f>
+        <v>784</v>
+      </c>
+      <c r="F40" s="2" t="n">
+        <f aca="false">4+E40</f>
+        <v>788</v>
+      </c>
+      <c r="G40" s="2" t="n">
+        <f aca="false">4+F40</f>
+        <v>792</v>
+      </c>
+      <c r="H40" s="2" t="n">
+        <f aca="false">4+G40</f>
+        <v>796</v>
+      </c>
+      <c r="I40" s="2" t="n">
+        <f aca="false">4+H40</f>
+        <v>800</v>
+      </c>
+      <c r="J40" s="2" t="n">
+        <f aca="false">4+I40</f>
+        <v>804</v>
+      </c>
+      <c r="K40" s="2" t="n">
+        <f aca="false">4+J40</f>
+        <v>808</v>
+      </c>
+      <c r="L40" s="2" t="n">
+        <f aca="false">4+K40</f>
+        <v>812</v>
+      </c>
+      <c r="M40" s="2" t="n">
+        <f aca="false">4+L40</f>
+        <v>816</v>
+      </c>
+      <c r="N40" s="2" t="n">
+        <f aca="false">4+M40</f>
+        <v>820</v>
+      </c>
+      <c r="O40" s="4" t="n">
+        <f aca="false">4+N40</f>
+        <v>824</v>
+      </c>
+      <c r="P40" s="2" t="n">
+        <f aca="false">4+O40</f>
+        <v>828</v>
+      </c>
+      <c r="Q40" s="2" t="n">
+        <f aca="false">4+P40</f>
+        <v>832</v>
+      </c>
+      <c r="R40" s="2" t="n">
+        <f aca="false">4+Q40</f>
+        <v>836</v>
+      </c>
+      <c r="S40" s="2" t="n">
+        <f aca="false">4+R40</f>
+        <v>840</v>
+      </c>
+      <c r="T40" s="2" t="n">
+        <f aca="false">4+S40</f>
+        <v>844</v>
+      </c>
+      <c r="U40" s="2" t="n">
+        <f aca="false">4+T40</f>
+        <v>848</v>
+      </c>
+      <c r="V40" s="2" t="n">
+        <f aca="false">4+U40</f>
+        <v>852</v>
+      </c>
+      <c r="W40" s="2" t="n">
+        <f aca="false">4+V40</f>
+        <v>856</v>
+      </c>
+      <c r="X40" s="2" t="n">
+        <f aca="false">4+W40</f>
+        <v>860</v>
+      </c>
+      <c r="Y40" s="2" t="n">
+        <f aca="false">4+X40</f>
+        <v>864</v>
+      </c>
+      <c r="Z40" s="2" t="n">
+        <f aca="false">4+Y40</f>
+        <v>868</v>
+      </c>
+      <c r="AA40" s="2" t="n">
+        <f aca="false">4+Z40</f>
+        <v>872</v>
+      </c>
+      <c r="AB40" s="2" t="n">
+        <f aca="false">4+AA40</f>
+        <v>876</v>
+      </c>
+      <c r="AC40" s="2" t="n">
+        <f aca="false">4+AB40</f>
+        <v>880</v>
+      </c>
+      <c r="AD40" s="2" t="n">
+        <f aca="false">4+AC40</f>
+        <v>884</v>
+      </c>
+      <c r="AE40" s="2" t="n">
+        <f aca="false">4+AD40</f>
+        <v>888</v>
+      </c>
+      <c r="AF40" s="2" t="n">
+        <f aca="false">4+AE40</f>
+        <v>892</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="47.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A41" s="2" t="n">
+        <f aca="false">128+A40</f>
+        <v>896</v>
+      </c>
+      <c r="B41" s="4" t="n">
+        <f aca="false">4+A41</f>
+        <v>900</v>
+      </c>
+      <c r="C41" s="2" t="n">
+        <f aca="false">4+B41</f>
+        <v>904</v>
+      </c>
+      <c r="D41" s="2" t="n">
+        <f aca="false">4+C41</f>
+        <v>908</v>
+      </c>
+      <c r="E41" s="2" t="n">
+        <f aca="false">4+D41</f>
+        <v>912</v>
+      </c>
+      <c r="F41" s="2" t="n">
+        <f aca="false">4+E41</f>
+        <v>916</v>
+      </c>
+      <c r="G41" s="2" t="n">
+        <f aca="false">4+F41</f>
+        <v>920</v>
+      </c>
+      <c r="H41" s="2" t="n">
+        <f aca="false">4+G41</f>
+        <v>924</v>
+      </c>
+      <c r="I41" s="2" t="n">
+        <f aca="false">4+H41</f>
+        <v>928</v>
+      </c>
+      <c r="J41" s="2" t="n">
+        <f aca="false">4+I41</f>
+        <v>932</v>
+      </c>
+      <c r="K41" s="2" t="n">
+        <f aca="false">4+J41</f>
+        <v>936</v>
+      </c>
+      <c r="L41" s="2" t="n">
+        <f aca="false">4+K41</f>
+        <v>940</v>
+      </c>
+      <c r="M41" s="2" t="n">
+        <f aca="false">4+L41</f>
+        <v>944</v>
+      </c>
+      <c r="N41" s="2" t="n">
+        <f aca="false">4+M41</f>
+        <v>948</v>
+      </c>
+      <c r="O41" s="4" t="n">
+        <f aca="false">4+N41</f>
+        <v>952</v>
+      </c>
+      <c r="P41" s="2" t="n">
+        <f aca="false">4+O41</f>
+        <v>956</v>
+      </c>
+      <c r="Q41" s="2" t="n">
+        <f aca="false">4+P41</f>
+        <v>960</v>
+      </c>
+      <c r="R41" s="2" t="n">
+        <f aca="false">4+Q41</f>
+        <v>964</v>
+      </c>
+      <c r="S41" s="2" t="n">
+        <f aca="false">4+R41</f>
+        <v>968</v>
+      </c>
+      <c r="T41" s="2" t="n">
+        <f aca="false">4+S41</f>
+        <v>972</v>
+      </c>
+      <c r="U41" s="2" t="n">
+        <f aca="false">4+T41</f>
+        <v>976</v>
+      </c>
+      <c r="V41" s="2" t="n">
+        <f aca="false">4+U41</f>
+        <v>980</v>
+      </c>
+      <c r="W41" s="2" t="n">
+        <f aca="false">4+V41</f>
+        <v>984</v>
+      </c>
+      <c r="X41" s="2" t="n">
+        <f aca="false">4+W41</f>
+        <v>988</v>
+      </c>
+      <c r="Y41" s="2" t="n">
+        <f aca="false">4+X41</f>
+        <v>992</v>
+      </c>
+      <c r="Z41" s="2" t="n">
+        <f aca="false">4+Y41</f>
+        <v>996</v>
+      </c>
+      <c r="AA41" s="2" t="n">
+        <f aca="false">4+Z41</f>
+        <v>1000</v>
+      </c>
+      <c r="AB41" s="2" t="n">
+        <f aca="false">4+AA41</f>
+        <v>1004</v>
+      </c>
+      <c r="AC41" s="2" t="n">
+        <f aca="false">4+AB41</f>
+        <v>1008</v>
+      </c>
+      <c r="AD41" s="2" t="n">
+        <f aca="false">4+AC41</f>
+        <v>1012</v>
+      </c>
+      <c r="AE41" s="2" t="n">
+        <f aca="false">4+AD41</f>
+        <v>1016</v>
+      </c>
+      <c r="AF41" s="2" t="n">
+        <f aca="false">4+AE41</f>
+        <v>1020</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="47.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A42" s="2" t="n">
+        <f aca="false">128+A41</f>
+        <v>1024</v>
+      </c>
+      <c r="B42" s="4" t="n">
+        <f aca="false">4+A42</f>
+        <v>1028</v>
+      </c>
+      <c r="C42" s="2" t="n">
+        <f aca="false">4+B42</f>
+        <v>1032</v>
+      </c>
+      <c r="D42" s="2" t="n">
+        <f aca="false">4+C42</f>
+        <v>1036</v>
+      </c>
+      <c r="E42" s="2" t="n">
+        <f aca="false">4+D42</f>
+        <v>1040</v>
+      </c>
+      <c r="F42" s="2" t="n">
+        <f aca="false">4+E42</f>
+        <v>1044</v>
+      </c>
+      <c r="G42" s="2" t="n">
+        <f aca="false">4+F42</f>
+        <v>1048</v>
+      </c>
+      <c r="H42" s="2" t="n">
+        <f aca="false">4+G42</f>
+        <v>1052</v>
+      </c>
+      <c r="I42" s="2" t="n">
+        <f aca="false">4+H42</f>
+        <v>1056</v>
+      </c>
+      <c r="J42" s="2" t="n">
+        <f aca="false">4+I42</f>
+        <v>1060</v>
+      </c>
+      <c r="K42" s="2" t="n">
+        <f aca="false">4+J42</f>
+        <v>1064</v>
+      </c>
+      <c r="L42" s="2" t="n">
+        <f aca="false">4+K42</f>
+        <v>1068</v>
+      </c>
+      <c r="M42" s="2" t="n">
+        <f aca="false">4+L42</f>
+        <v>1072</v>
+      </c>
+      <c r="N42" s="2" t="n">
+        <f aca="false">4+M42</f>
+        <v>1076</v>
+      </c>
+      <c r="O42" s="4" t="n">
+        <f aca="false">4+N42</f>
+        <v>1080</v>
+      </c>
+      <c r="P42" s="2" t="n">
+        <f aca="false">4+O42</f>
+        <v>1084</v>
+      </c>
+      <c r="Q42" s="2" t="n">
+        <f aca="false">4+P42</f>
+        <v>1088</v>
+      </c>
+      <c r="R42" s="2" t="n">
+        <f aca="false">4+Q42</f>
+        <v>1092</v>
+      </c>
+      <c r="S42" s="2" t="n">
+        <f aca="false">4+R42</f>
+        <v>1096</v>
+      </c>
+      <c r="T42" s="2" t="n">
+        <f aca="false">4+S42</f>
+        <v>1100</v>
+      </c>
+      <c r="U42" s="2" t="n">
+        <f aca="false">4+T42</f>
+        <v>1104</v>
+      </c>
+      <c r="V42" s="2" t="n">
+        <f aca="false">4+U42</f>
+        <v>1108</v>
+      </c>
+      <c r="W42" s="2" t="n">
+        <f aca="false">4+V42</f>
+        <v>1112</v>
+      </c>
+      <c r="X42" s="2" t="n">
+        <f aca="false">4+W42</f>
+        <v>1116</v>
+      </c>
+      <c r="Y42" s="2" t="n">
+        <f aca="false">4+X42</f>
+        <v>1120</v>
+      </c>
+      <c r="Z42" s="2" t="n">
+        <f aca="false">4+Y42</f>
+        <v>1124</v>
+      </c>
+      <c r="AA42" s="2" t="n">
+        <f aca="false">4+Z42</f>
+        <v>1128</v>
+      </c>
+      <c r="AB42" s="2" t="n">
+        <f aca="false">4+AA42</f>
+        <v>1132</v>
+      </c>
+      <c r="AC42" s="2" t="n">
+        <f aca="false">4+AB42</f>
+        <v>1136</v>
+      </c>
+      <c r="AD42" s="2" t="n">
+        <f aca="false">4+AC42</f>
+        <v>1140</v>
+      </c>
+      <c r="AE42" s="2" t="n">
+        <f aca="false">4+AD42</f>
+        <v>1144</v>
+      </c>
+      <c r="AF42" s="2" t="n">
+        <f aca="false">4+AE42</f>
+        <v>1148</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="47.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A43" s="2" t="n">
+        <f aca="false">128+A42</f>
+        <v>1152</v>
+      </c>
+      <c r="B43" s="4" t="n">
+        <f aca="false">4+A43</f>
+        <v>1156</v>
+      </c>
+      <c r="C43" s="2" t="n">
+        <f aca="false">4+B43</f>
+        <v>1160</v>
+      </c>
+      <c r="D43" s="2" t="n">
+        <f aca="false">4+C43</f>
+        <v>1164</v>
+      </c>
+      <c r="E43" s="2" t="n">
+        <f aca="false">4+D43</f>
+        <v>1168</v>
+      </c>
+      <c r="F43" s="2" t="n">
+        <f aca="false">4+E43</f>
+        <v>1172</v>
+      </c>
+      <c r="G43" s="2" t="n">
+        <f aca="false">4+F43</f>
+        <v>1176</v>
+      </c>
+      <c r="H43" s="2" t="n">
+        <f aca="false">4+G43</f>
+        <v>1180</v>
+      </c>
+      <c r="I43" s="2" t="n">
+        <f aca="false">4+H43</f>
+        <v>1184</v>
+      </c>
+      <c r="J43" s="2" t="n">
+        <f aca="false">4+I43</f>
+        <v>1188</v>
+      </c>
+      <c r="K43" s="2" t="n">
+        <f aca="false">4+J43</f>
+        <v>1192</v>
+      </c>
+      <c r="L43" s="2" t="n">
+        <f aca="false">4+K43</f>
+        <v>1196</v>
+      </c>
+      <c r="M43" s="2" t="n">
+        <f aca="false">4+L43</f>
+        <v>1200</v>
+      </c>
+      <c r="N43" s="2" t="n">
+        <f aca="false">4+M43</f>
+        <v>1204</v>
+      </c>
+      <c r="O43" s="4" t="n">
+        <f aca="false">4+N43</f>
+        <v>1208</v>
+      </c>
+      <c r="P43" s="2" t="n">
+        <f aca="false">4+O43</f>
+        <v>1212</v>
+      </c>
+      <c r="Q43" s="2" t="n">
+        <f aca="false">4+P43</f>
+        <v>1216</v>
+      </c>
+      <c r="R43" s="2" t="n">
+        <f aca="false">4+Q43</f>
+        <v>1220</v>
+      </c>
+      <c r="S43" s="2" t="n">
+        <f aca="false">4+R43</f>
+        <v>1224</v>
+      </c>
+      <c r="T43" s="2" t="n">
+        <f aca="false">4+S43</f>
+        <v>1228</v>
+      </c>
+      <c r="U43" s="2" t="n">
+        <f aca="false">4+T43</f>
+        <v>1232</v>
+      </c>
+      <c r="V43" s="2" t="n">
+        <f aca="false">4+U43</f>
+        <v>1236</v>
+      </c>
+      <c r="W43" s="2" t="n">
+        <f aca="false">4+V43</f>
+        <v>1240</v>
+      </c>
+      <c r="X43" s="2" t="n">
+        <f aca="false">4+W43</f>
+        <v>1244</v>
+      </c>
+      <c r="Y43" s="2" t="n">
+        <f aca="false">4+X43</f>
+        <v>1248</v>
+      </c>
+      <c r="Z43" s="2" t="n">
+        <f aca="false">4+Y43</f>
+        <v>1252</v>
+      </c>
+      <c r="AA43" s="2" t="n">
+        <f aca="false">4+Z43</f>
+        <v>1256</v>
+      </c>
+      <c r="AB43" s="2" t="n">
+        <f aca="false">4+AA43</f>
+        <v>1260</v>
+      </c>
+      <c r="AC43" s="2" t="n">
+        <f aca="false">4+AB43</f>
+        <v>1264</v>
+      </c>
+      <c r="AD43" s="2" t="n">
+        <f aca="false">4+AC43</f>
+        <v>1268</v>
+      </c>
+      <c r="AE43" s="2" t="n">
+        <f aca="false">4+AD43</f>
+        <v>1272</v>
+      </c>
+      <c r="AF43" s="2" t="n">
+        <f aca="false">4+AE43</f>
+        <v>1276</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="47.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A44" s="2" t="n">
+        <f aca="false">128+A43</f>
+        <v>1280</v>
+      </c>
+      <c r="B44" s="4" t="n">
+        <f aca="false">4+A44</f>
+        <v>1284</v>
+      </c>
+      <c r="C44" s="2" t="n">
+        <f aca="false">4+B44</f>
+        <v>1288</v>
+      </c>
+      <c r="D44" s="2" t="n">
+        <f aca="false">4+C44</f>
+        <v>1292</v>
+      </c>
+      <c r="E44" s="2" t="n">
+        <f aca="false">4+D44</f>
+        <v>1296</v>
+      </c>
+      <c r="F44" s="2" t="n">
+        <f aca="false">4+E44</f>
+        <v>1300</v>
+      </c>
+      <c r="G44" s="2" t="n">
+        <f aca="false">4+F44</f>
+        <v>1304</v>
+      </c>
+      <c r="H44" s="2" t="n">
+        <f aca="false">4+G44</f>
+        <v>1308</v>
+      </c>
+      <c r="I44" s="2" t="n">
+        <f aca="false">4+H44</f>
+        <v>1312</v>
+      </c>
+      <c r="J44" s="2" t="n">
+        <f aca="false">4+I44</f>
+        <v>1316</v>
+      </c>
+      <c r="K44" s="2" t="n">
+        <f aca="false">4+J44</f>
+        <v>1320</v>
+      </c>
+      <c r="L44" s="2" t="n">
+        <f aca="false">4+K44</f>
+        <v>1324</v>
+      </c>
+      <c r="M44" s="2" t="n">
+        <f aca="false">4+L44</f>
+        <v>1328</v>
+      </c>
+      <c r="N44" s="2" t="n">
+        <f aca="false">4+M44</f>
+        <v>1332</v>
+      </c>
+      <c r="O44" s="4" t="n">
+        <f aca="false">4+N44</f>
+        <v>1336</v>
+      </c>
+      <c r="P44" s="2" t="n">
+        <f aca="false">4+O44</f>
+        <v>1340</v>
+      </c>
+      <c r="Q44" s="2" t="n">
+        <f aca="false">4+P44</f>
+        <v>1344</v>
+      </c>
+      <c r="R44" s="2" t="n">
+        <f aca="false">4+Q44</f>
+        <v>1348</v>
+      </c>
+      <c r="S44" s="2" t="n">
+        <f aca="false">4+R44</f>
+        <v>1352</v>
+      </c>
+      <c r="T44" s="2" t="n">
+        <f aca="false">4+S44</f>
+        <v>1356</v>
+      </c>
+      <c r="U44" s="2" t="n">
+        <f aca="false">4+T44</f>
+        <v>1360</v>
+      </c>
+      <c r="V44" s="2" t="n">
+        <f aca="false">4+U44</f>
+        <v>1364</v>
+      </c>
+      <c r="W44" s="2" t="n">
+        <f aca="false">4+V44</f>
+        <v>1368</v>
+      </c>
+      <c r="X44" s="2" t="n">
+        <f aca="false">4+W44</f>
+        <v>1372</v>
+      </c>
+      <c r="Y44" s="2" t="n">
+        <f aca="false">4+X44</f>
+        <v>1376</v>
+      </c>
+      <c r="Z44" s="2" t="n">
+        <f aca="false">4+Y44</f>
+        <v>1380</v>
+      </c>
+      <c r="AA44" s="2" t="n">
+        <f aca="false">4+Z44</f>
+        <v>1384</v>
+      </c>
+      <c r="AB44" s="2" t="n">
+        <f aca="false">4+AA44</f>
+        <v>1388</v>
+      </c>
+      <c r="AC44" s="2" t="n">
+        <f aca="false">4+AB44</f>
+        <v>1392</v>
+      </c>
+      <c r="AD44" s="2" t="n">
+        <f aca="false">4+AC44</f>
+        <v>1396</v>
+      </c>
+      <c r="AE44" s="2" t="n">
+        <f aca="false">4+AD44</f>
+        <v>1400</v>
+      </c>
+      <c r="AF44" s="2" t="n">
+        <f aca="false">4+AE44</f>
+        <v>1404</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="47.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A45" s="2" t="n">
+        <f aca="false">128+A44</f>
+        <v>1408</v>
+      </c>
+      <c r="B45" s="4" t="n">
+        <f aca="false">4+A45</f>
+        <v>1412</v>
+      </c>
+      <c r="C45" s="2" t="n">
+        <f aca="false">4+B45</f>
+        <v>1416</v>
+      </c>
+      <c r="D45" s="2" t="n">
+        <f aca="false">4+C45</f>
+        <v>1420</v>
+      </c>
+      <c r="E45" s="2" t="n">
+        <f aca="false">4+D45</f>
+        <v>1424</v>
+      </c>
+      <c r="F45" s="2" t="n">
+        <f aca="false">4+E45</f>
+        <v>1428</v>
+      </c>
+      <c r="G45" s="2" t="n">
+        <f aca="false">4+F45</f>
+        <v>1432</v>
+      </c>
+      <c r="H45" s="2" t="n">
+        <f aca="false">4+G45</f>
+        <v>1436</v>
+      </c>
+      <c r="I45" s="2" t="n">
+        <f aca="false">4+H45</f>
+        <v>1440</v>
+      </c>
+      <c r="J45" s="2" t="n">
+        <f aca="false">4+I45</f>
+        <v>1444</v>
+      </c>
+      <c r="K45" s="2" t="n">
+        <f aca="false">4+J45</f>
+        <v>1448</v>
+      </c>
+      <c r="L45" s="2" t="n">
+        <f aca="false">4+K45</f>
+        <v>1452</v>
+      </c>
+      <c r="M45" s="2" t="n">
+        <f aca="false">4+L45</f>
+        <v>1456</v>
+      </c>
+      <c r="N45" s="2" t="n">
+        <f aca="false">4+M45</f>
+        <v>1460</v>
+      </c>
+      <c r="O45" s="4" t="n">
+        <f aca="false">4+N45</f>
+        <v>1464</v>
+      </c>
+      <c r="P45" s="2" t="n">
+        <f aca="false">4+O45</f>
+        <v>1468</v>
+      </c>
+      <c r="Q45" s="2" t="n">
+        <f aca="false">4+P45</f>
+        <v>1472</v>
+      </c>
+      <c r="R45" s="2" t="n">
+        <f aca="false">4+Q45</f>
+        <v>1476</v>
+      </c>
+      <c r="S45" s="2" t="n">
+        <f aca="false">4+R45</f>
+        <v>1480</v>
+      </c>
+      <c r="T45" s="2" t="n">
+        <f aca="false">4+S45</f>
+        <v>1484</v>
+      </c>
+      <c r="U45" s="2" t="n">
+        <f aca="false">4+T45</f>
+        <v>1488</v>
+      </c>
+      <c r="V45" s="2" t="n">
+        <f aca="false">4+U45</f>
+        <v>1492</v>
+      </c>
+      <c r="W45" s="2" t="n">
+        <f aca="false">4+V45</f>
+        <v>1496</v>
+      </c>
+      <c r="X45" s="2" t="n">
+        <f aca="false">4+W45</f>
+        <v>1500</v>
+      </c>
+      <c r="Y45" s="2" t="n">
+        <f aca="false">4+X45</f>
+        <v>1504</v>
+      </c>
+      <c r="Z45" s="2" t="n">
+        <f aca="false">4+Y45</f>
+        <v>1508</v>
+      </c>
+      <c r="AA45" s="2" t="n">
+        <f aca="false">4+Z45</f>
+        <v>1512</v>
+      </c>
+      <c r="AB45" s="2" t="n">
+        <f aca="false">4+AA45</f>
+        <v>1516</v>
+      </c>
+      <c r="AC45" s="2" t="n">
+        <f aca="false">4+AB45</f>
+        <v>1520</v>
+      </c>
+      <c r="AD45" s="2" t="n">
+        <f aca="false">4+AC45</f>
+        <v>1524</v>
+      </c>
+      <c r="AE45" s="2" t="n">
+        <f aca="false">4+AD45</f>
+        <v>1528</v>
+      </c>
+      <c r="AF45" s="2" t="n">
+        <f aca="false">4+AE45</f>
+        <v>1532</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="47.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A46" s="2" t="n">
+        <f aca="false">128+A45</f>
+        <v>1536</v>
+      </c>
+      <c r="B46" s="4" t="n">
+        <f aca="false">4+A46</f>
+        <v>1540</v>
+      </c>
+      <c r="C46" s="2" t="n">
+        <f aca="false">4+B46</f>
+        <v>1544</v>
+      </c>
+      <c r="D46" s="2" t="n">
+        <f aca="false">4+C46</f>
+        <v>1548</v>
+      </c>
+      <c r="E46" s="2" t="n">
+        <f aca="false">4+D46</f>
+        <v>1552</v>
+      </c>
+      <c r="F46" s="2" t="n">
+        <f aca="false">4+E46</f>
+        <v>1556</v>
+      </c>
+      <c r="G46" s="2" t="n">
+        <f aca="false">4+F46</f>
+        <v>1560</v>
+      </c>
+      <c r="H46" s="2" t="n">
+        <f aca="false">4+G46</f>
+        <v>1564</v>
+      </c>
+      <c r="I46" s="2" t="n">
+        <f aca="false">4+H46</f>
+        <v>1568</v>
+      </c>
+      <c r="J46" s="2" t="n">
+        <f aca="false">4+I46</f>
+        <v>1572</v>
+      </c>
+      <c r="K46" s="2" t="n">
+        <f aca="false">4+J46</f>
+        <v>1576</v>
+      </c>
+      <c r="L46" s="2" t="n">
+        <f aca="false">4+K46</f>
+        <v>1580</v>
+      </c>
+      <c r="M46" s="2" t="n">
+        <f aca="false">4+L46</f>
+        <v>1584</v>
+      </c>
+      <c r="N46" s="2" t="n">
+        <f aca="false">4+M46</f>
+        <v>1588</v>
+      </c>
+      <c r="O46" s="4" t="n">
+        <f aca="false">4+N46</f>
+        <v>1592</v>
+      </c>
+      <c r="P46" s="2" t="n">
+        <f aca="false">4+O46</f>
+        <v>1596</v>
+      </c>
+      <c r="Q46" s="2" t="n">
+        <f aca="false">4+P46</f>
+        <v>1600</v>
+      </c>
+      <c r="R46" s="2" t="n">
+        <f aca="false">4+Q46</f>
+        <v>1604</v>
+      </c>
+      <c r="S46" s="2" t="n">
+        <f aca="false">4+R46</f>
+        <v>1608</v>
+      </c>
+      <c r="T46" s="2" t="n">
+        <f aca="false">4+S46</f>
+        <v>1612</v>
+      </c>
+      <c r="U46" s="2" t="n">
+        <f aca="false">4+T46</f>
+        <v>1616</v>
+      </c>
+      <c r="V46" s="2" t="n">
+        <f aca="false">4+U46</f>
+        <v>1620</v>
+      </c>
+      <c r="W46" s="2" t="n">
+        <f aca="false">4+V46</f>
+        <v>1624</v>
+      </c>
+      <c r="X46" s="2" t="n">
+        <f aca="false">4+W46</f>
+        <v>1628</v>
+      </c>
+      <c r="Y46" s="2" t="n">
+        <f aca="false">4+X46</f>
+        <v>1632</v>
+      </c>
+      <c r="Z46" s="2" t="n">
+        <f aca="false">4+Y46</f>
+        <v>1636</v>
+      </c>
+      <c r="AA46" s="2" t="n">
+        <f aca="false">4+Z46</f>
+        <v>1640</v>
+      </c>
+      <c r="AB46" s="2" t="n">
+        <f aca="false">4+AA46</f>
+        <v>1644</v>
+      </c>
+      <c r="AC46" s="2" t="n">
+        <f aca="false">4+AB46</f>
+        <v>1648</v>
+      </c>
+      <c r="AD46" s="2" t="n">
+        <f aca="false">4+AC46</f>
+        <v>1652</v>
+      </c>
+      <c r="AE46" s="2" t="n">
+        <f aca="false">4+AD46</f>
+        <v>1656</v>
+      </c>
+      <c r="AF46" s="2" t="n">
+        <f aca="false">4+AE46</f>
+        <v>1660</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="47.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A47" s="2" t="n">
+        <f aca="false">128+A46</f>
+        <v>1664</v>
+      </c>
+      <c r="B47" s="4" t="n">
+        <f aca="false">4+A47</f>
+        <v>1668</v>
+      </c>
+      <c r="C47" s="2" t="n">
+        <f aca="false">4+B47</f>
+        <v>1672</v>
+      </c>
+      <c r="D47" s="2" t="n">
+        <f aca="false">4+C47</f>
+        <v>1676</v>
+      </c>
+      <c r="E47" s="2" t="n">
+        <f aca="false">4+D47</f>
+        <v>1680</v>
+      </c>
+      <c r="F47" s="2" t="n">
+        <f aca="false">4+E47</f>
+        <v>1684</v>
+      </c>
+      <c r="G47" s="2" t="n">
+        <f aca="false">4+F47</f>
+        <v>1688</v>
+      </c>
+      <c r="H47" s="2" t="n">
+        <f aca="false">4+G47</f>
+        <v>1692</v>
+      </c>
+      <c r="I47" s="2" t="n">
+        <f aca="false">4+H47</f>
+        <v>1696</v>
+      </c>
+      <c r="J47" s="2" t="n">
+        <f aca="false">4+I47</f>
+        <v>1700</v>
+      </c>
+      <c r="K47" s="2" t="n">
+        <f aca="false">4+J47</f>
+        <v>1704</v>
+      </c>
+      <c r="L47" s="2" t="n">
+        <f aca="false">4+K47</f>
+        <v>1708</v>
+      </c>
+      <c r="M47" s="2" t="n">
+        <f aca="false">4+L47</f>
+        <v>1712</v>
+      </c>
+      <c r="N47" s="2" t="n">
+        <f aca="false">4+M47</f>
+        <v>1716</v>
+      </c>
+      <c r="O47" s="4" t="n">
+        <f aca="false">4+N47</f>
+        <v>1720</v>
+      </c>
+      <c r="P47" s="2" t="n">
+        <f aca="false">4+O47</f>
+        <v>1724</v>
+      </c>
+      <c r="Q47" s="2" t="n">
+        <f aca="false">4+P47</f>
+        <v>1728</v>
+      </c>
+      <c r="R47" s="2" t="n">
+        <f aca="false">4+Q47</f>
+        <v>1732</v>
+      </c>
+      <c r="S47" s="2" t="n">
+        <f aca="false">4+R47</f>
+        <v>1736</v>
+      </c>
+      <c r="T47" s="2" t="n">
+        <f aca="false">4+S47</f>
+        <v>1740</v>
+      </c>
+      <c r="U47" s="2" t="n">
+        <f aca="false">4+T47</f>
+        <v>1744</v>
+      </c>
+      <c r="V47" s="2" t="n">
+        <f aca="false">4+U47</f>
+        <v>1748</v>
+      </c>
+      <c r="W47" s="2" t="n">
+        <f aca="false">4+V47</f>
+        <v>1752</v>
+      </c>
+      <c r="X47" s="2" t="n">
+        <f aca="false">4+W47</f>
+        <v>1756</v>
+      </c>
+      <c r="Y47" s="2" t="n">
+        <f aca="false">4+X47</f>
+        <v>1760</v>
+      </c>
+      <c r="Z47" s="2" t="n">
+        <f aca="false">4+Y47</f>
+        <v>1764</v>
+      </c>
+      <c r="AA47" s="2" t="n">
+        <f aca="false">4+Z47</f>
+        <v>1768</v>
+      </c>
+      <c r="AB47" s="2" t="n">
+        <f aca="false">4+AA47</f>
+        <v>1772</v>
+      </c>
+      <c r="AC47" s="2" t="n">
+        <f aca="false">4+AB47</f>
+        <v>1776</v>
+      </c>
+      <c r="AD47" s="2" t="n">
+        <f aca="false">4+AC47</f>
+        <v>1780</v>
+      </c>
+      <c r="AE47" s="2" t="n">
+        <f aca="false">4+AD47</f>
+        <v>1784</v>
+      </c>
+      <c r="AF47" s="2" t="n">
+        <f aca="false">4+AE47</f>
+        <v>1788</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="47.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A48" s="2" t="n">
+        <f aca="false">128+A47</f>
+        <v>1792</v>
+      </c>
+      <c r="B48" s="4" t="n">
+        <f aca="false">4+A48</f>
+        <v>1796</v>
+      </c>
+      <c r="C48" s="4" t="n">
+        <f aca="false">4+B48</f>
+        <v>1800</v>
+      </c>
+      <c r="D48" s="4" t="n">
+        <f aca="false">4+C48</f>
+        <v>1804</v>
+      </c>
+      <c r="E48" s="4" t="n">
+        <f aca="false">4+D48</f>
+        <v>1808</v>
+      </c>
+      <c r="F48" s="4" t="n">
+        <f aca="false">4+E48</f>
+        <v>1812</v>
+      </c>
+      <c r="G48" s="4" t="n">
+        <f aca="false">4+F48</f>
+        <v>1816</v>
+      </c>
+      <c r="H48" s="4" t="n">
+        <f aca="false">4+G48</f>
+        <v>1820</v>
+      </c>
+      <c r="I48" s="4" t="n">
+        <f aca="false">4+H48</f>
+        <v>1824</v>
+      </c>
+      <c r="J48" s="4" t="n">
+        <f aca="false">4+I48</f>
+        <v>1828</v>
+      </c>
+      <c r="K48" s="4" t="n">
+        <f aca="false">4+J48</f>
+        <v>1832</v>
+      </c>
+      <c r="L48" s="4" t="n">
+        <f aca="false">4+K48</f>
+        <v>1836</v>
+      </c>
+      <c r="M48" s="4" t="n">
+        <f aca="false">4+L48</f>
+        <v>1840</v>
+      </c>
+      <c r="N48" s="4" t="n">
+        <f aca="false">4+M48</f>
+        <v>1844</v>
+      </c>
+      <c r="O48" s="4" t="n">
+        <f aca="false">4+N48</f>
+        <v>1848</v>
+      </c>
+      <c r="P48" s="2" t="n">
+        <f aca="false">4+O48</f>
+        <v>1852</v>
+      </c>
+      <c r="Q48" s="2" t="n">
+        <f aca="false">4+P48</f>
+        <v>1856</v>
+      </c>
+      <c r="R48" s="2" t="n">
+        <f aca="false">4+Q48</f>
+        <v>1860</v>
+      </c>
+      <c r="S48" s="2" t="n">
+        <f aca="false">4+R48</f>
+        <v>1864</v>
+      </c>
+      <c r="T48" s="2" t="n">
+        <f aca="false">4+S48</f>
+        <v>1868</v>
+      </c>
+      <c r="U48" s="2" t="n">
+        <f aca="false">4+T48</f>
+        <v>1872</v>
+      </c>
+      <c r="V48" s="2" t="n">
+        <f aca="false">4+U48</f>
+        <v>1876</v>
+      </c>
+      <c r="W48" s="2" t="n">
+        <f aca="false">4+V48</f>
+        <v>1880</v>
+      </c>
+      <c r="X48" s="2" t="n">
+        <f aca="false">4+W48</f>
+        <v>1884</v>
+      </c>
+      <c r="Y48" s="2" t="n">
+        <f aca="false">4+X48</f>
+        <v>1888</v>
+      </c>
+      <c r="Z48" s="2" t="n">
+        <f aca="false">4+Y48</f>
+        <v>1892</v>
+      </c>
+      <c r="AA48" s="2" t="n">
+        <f aca="false">4+Z48</f>
+        <v>1896</v>
+      </c>
+      <c r="AB48" s="2" t="n">
+        <f aca="false">4+AA48</f>
+        <v>1900</v>
+      </c>
+      <c r="AC48" s="2" t="n">
+        <f aca="false">4+AB48</f>
+        <v>1904</v>
+      </c>
+      <c r="AD48" s="2" t="n">
+        <f aca="false">4+AC48</f>
+        <v>1908</v>
+      </c>
+      <c r="AE48" s="2" t="n">
+        <f aca="false">4+AD48</f>
+        <v>1912</v>
+      </c>
+      <c r="AF48" s="2" t="n">
+        <f aca="false">4+AE48</f>
+        <v>1916</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="47.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A49" s="2" t="n">
+        <f aca="false">128+A48</f>
+        <v>1920</v>
+      </c>
+      <c r="B49" s="2" t="n">
+        <f aca="false">4+A49</f>
+        <v>1924</v>
+      </c>
+      <c r="C49" s="2" t="n">
+        <f aca="false">4+B49</f>
+        <v>1928</v>
+      </c>
+      <c r="D49" s="2" t="n">
+        <f aca="false">4+C49</f>
+        <v>1932</v>
+      </c>
+      <c r="E49" s="2" t="n">
+        <f aca="false">4+D49</f>
+        <v>1936</v>
+      </c>
+      <c r="F49" s="2" t="n">
+        <f aca="false">4+E49</f>
+        <v>1940</v>
+      </c>
+      <c r="G49" s="2" t="n">
+        <f aca="false">4+F49</f>
+        <v>1944</v>
+      </c>
+      <c r="H49" s="2" t="n">
+        <f aca="false">4+G49</f>
+        <v>1948</v>
+      </c>
+      <c r="I49" s="2" t="n">
+        <f aca="false">4+H49</f>
+        <v>1952</v>
+      </c>
+      <c r="J49" s="2" t="n">
+        <f aca="false">4+I49</f>
+        <v>1956</v>
+      </c>
+      <c r="K49" s="2" t="n">
+        <f aca="false">4+J49</f>
+        <v>1960</v>
+      </c>
+      <c r="L49" s="2" t="n">
+        <f aca="false">4+K49</f>
+        <v>1964</v>
+      </c>
+      <c r="M49" s="2" t="n">
+        <f aca="false">4+L49</f>
+        <v>1968</v>
+      </c>
+      <c r="N49" s="2" t="n">
+        <f aca="false">4+M49</f>
+        <v>1972</v>
+      </c>
+      <c r="O49" s="2" t="n">
+        <f aca="false">4+N49</f>
+        <v>1976</v>
+      </c>
+      <c r="P49" s="2" t="n">
+        <f aca="false">4+O49</f>
+        <v>1980</v>
+      </c>
+      <c r="Q49" s="2" t="n">
+        <f aca="false">4+P49</f>
+        <v>1984</v>
+      </c>
+      <c r="R49" s="2" t="n">
+        <f aca="false">4+Q49</f>
+        <v>1988</v>
+      </c>
+      <c r="S49" s="2" t="n">
+        <f aca="false">4+R49</f>
+        <v>1992</v>
+      </c>
+      <c r="T49" s="2" t="n">
+        <f aca="false">4+S49</f>
+        <v>1996</v>
+      </c>
+      <c r="U49" s="2" t="n">
+        <f aca="false">4+T49</f>
+        <v>2000</v>
+      </c>
+      <c r="V49" s="2" t="n">
+        <f aca="false">4+U49</f>
+        <v>2004</v>
+      </c>
+      <c r="W49" s="2" t="n">
+        <f aca="false">4+V49</f>
+        <v>2008</v>
+      </c>
+      <c r="X49" s="2" t="n">
+        <f aca="false">4+W49</f>
+        <v>2012</v>
+      </c>
+      <c r="Y49" s="2" t="n">
+        <f aca="false">4+X49</f>
+        <v>2016</v>
+      </c>
+      <c r="Z49" s="2" t="n">
+        <f aca="false">4+Y49</f>
+        <v>2020</v>
+      </c>
+      <c r="AA49" s="2" t="n">
+        <f aca="false">4+Z49</f>
+        <v>2024</v>
+      </c>
+      <c r="AB49" s="2" t="n">
+        <f aca="false">4+AA49</f>
+        <v>2028</v>
+      </c>
+      <c r="AC49" s="2" t="n">
+        <f aca="false">4+AB49</f>
+        <v>2032</v>
+      </c>
+      <c r="AD49" s="2" t="n">
+        <f aca="false">4+AC49</f>
+        <v>2036</v>
+      </c>
+      <c r="AE49" s="2" t="n">
+        <f aca="false">4+AD49</f>
+        <v>2040</v>
+      </c>
+      <c r="AF49" s="2" t="n">
+        <f aca="false">4+AE49</f>
+        <v>2044</v>
       </c>
     </row>
   </sheetData>

</xml_diff>